<commit_message>
Removing maximal and final dimensions of the organs calculated by elong-wheat
</commit_message>
<xml_diff>
--- a/example/Vegetative_stages/inputs/Generate_inputs.xlsx
+++ b/example/Vegetative_stages/inputs/Generate_inputs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mngauthier\Documents\Marion_These\Modeles\fspm-wheat\trunk\example\Vegetative_stages\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CN-Wheat\fspm-wheat\example\Vegetative_stages\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7320" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INPUTS" sheetId="15" r:id="rId1"/>
@@ -92,7 +92,7 @@
     <author>mngauthier</author>
   </authors>
   <commentList>
-    <comment ref="AR7" authorId="0" shapeId="0">
+    <comment ref="AT7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -179,7 +179,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="182">
   <si>
     <t>plant</t>
   </si>
@@ -830,6 +830,12 @@
   </si>
   <si>
     <t>g.m-3</t>
+  </si>
+  <si>
+    <t>mstruct_eqL4</t>
+  </si>
+  <si>
+    <t>mstruct_eqL3</t>
   </si>
 </sst>
 </file>
@@ -1008,7 +1014,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1018,6 +1024,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1251,7 +1263,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1414,6 +1426,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1704,19 +1717,19 @@
       <selection activeCell="AO1" sqref="AO1:AO1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.85546875" customWidth="1"/>
-    <col min="35" max="35" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.88671875" customWidth="1"/>
+    <col min="35" max="35" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="12" bestFit="1" customWidth="1"/>
     <col min="46" max="47" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A1" s="49" t="s">
         <v>112</v>
       </c>
@@ -1734,7 +1747,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:55" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:55" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="52" t="s">
         <v>112</v>
       </c>
@@ -1753,7 +1766,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="4" spans="1:55" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:55" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="98" t="s">
         <v>70</v>
       </c>
@@ -1918,7 +1931,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A5" s="98"/>
       <c r="B5">
         <v>1</v>
@@ -2106,7 +2119,7 @@
         <v>1.3244862745926676E-6</v>
       </c>
     </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A6" s="98"/>
       <c r="B6">
         <v>1</v>
@@ -2293,7 +2306,7 @@
         <v>1.6879744031468265E-7</v>
       </c>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A7" s="98"/>
       <c r="B7">
         <v>1</v>
@@ -2477,7 +2490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A8" s="98"/>
       <c r="B8">
         <v>1</v>
@@ -2661,7 +2674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A9" s="98"/>
       <c r="B9">
         <v>1</v>
@@ -2845,7 +2858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A10" s="98"/>
       <c r="B10">
         <v>1</v>
@@ -3029,7 +3042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A11" s="98"/>
       <c r="B11">
         <v>1</v>
@@ -3213,7 +3226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A12" s="98"/>
       <c r="B12">
         <v>1</v>
@@ -3397,7 +3410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
@@ -3409,7 +3422,7 @@
       <c r="AE13" s="1"/>
       <c r="AF13" s="1"/>
     </row>
-    <row r="14" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="98" t="s">
         <v>71</v>
       </c>
@@ -3510,7 +3523,7 @@
       <c r="AT14" s="40"/>
       <c r="AU14" s="40"/>
     </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A15" s="98"/>
       <c r="B15">
         <v>1</v>
@@ -3633,7 +3646,7 @@
       <c r="AT15" s="83"/>
       <c r="AU15" s="83"/>
     </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A16" s="98"/>
       <c r="B16">
         <v>1</v>
@@ -3758,7 +3771,7 @@
       <c r="AT16" s="84"/>
       <c r="AU16" s="84"/>
     </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A17" s="98"/>
       <c r="B17">
         <v>1</v>
@@ -3862,7 +3875,7 @@
       <c r="AF17" s="1"/>
       <c r="AG17" s="1"/>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A18" s="98"/>
       <c r="B18">
         <v>1</v>
@@ -3966,7 +3979,7 @@
       <c r="AF18" s="1"/>
       <c r="AG18" s="1"/>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A19" s="98"/>
       <c r="B19">
         <v>1</v>
@@ -4075,7 +4088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A20" s="98"/>
       <c r="B20">
         <v>1</v>
@@ -4179,7 +4192,7 @@
         <v>0.106</v>
       </c>
     </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="V21" s="79"/>
       <c r="W21" s="15"/>
@@ -4200,7 +4213,7 @@
         <v>1.28</v>
       </c>
     </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="V22" s="29"/>
       <c r="W22" s="80"/>
@@ -4228,7 +4241,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="X23" s="14">
         <v>0.1</v>
@@ -4256,7 +4269,7 @@
         <v>1512000</v>
       </c>
     </row>
-    <row r="24" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -4275,7 +4288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A25" s="98" t="s">
         <v>72</v>
       </c>
@@ -4331,7 +4344,7 @@
         <v>1.6949152542372881E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A26" s="98"/>
       <c r="B26">
         <v>1</v>
@@ -4380,7 +4393,7 @@
       <c r="AU26" s="7"/>
       <c r="AV26" s="7"/>
     </row>
-    <row r="27" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A27" s="98"/>
       <c r="B27">
         <v>1</v>
@@ -4456,7 +4469,7 @@
       <c r="AU27" s="7"/>
       <c r="AV27" s="7"/>
     </row>
-    <row r="28" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:50" x14ac:dyDescent="0.3">
       <c r="E28" s="46">
         <f>AB16</f>
         <v>4411.7647058823532</v>
@@ -4510,7 +4523,7 @@
       <c r="AU28" s="7"/>
       <c r="AV28" s="7"/>
     </row>
-    <row r="29" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:50" x14ac:dyDescent="0.3">
       <c r="F29" s="1"/>
       <c r="R29" s="99"/>
       <c r="S29" s="7" t="s">
@@ -4538,7 +4551,7 @@
       <c r="AU29" s="7"/>
       <c r="AV29" s="7"/>
     </row>
-    <row r="30" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:50" x14ac:dyDescent="0.3">
       <c r="D30" s="23" t="s">
         <v>78</v>
       </c>
@@ -4574,7 +4587,7 @@
       <c r="AU30" s="7"/>
       <c r="AV30" s="7"/>
     </row>
-    <row r="31" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:50" x14ac:dyDescent="0.3">
       <c r="D31" s="20" t="s">
         <v>79</v>
       </c>
@@ -4621,7 +4634,7 @@
       <c r="AU31" s="7"/>
       <c r="AV31" s="7"/>
     </row>
-    <row r="32" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:50" x14ac:dyDescent="0.3">
       <c r="D32" s="20" t="s">
         <v>76</v>
       </c>
@@ -4655,7 +4668,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="O33" s="30" t="s">
         <v>108</v>
       </c>
@@ -4670,7 +4683,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
       <c r="O34" s="30" t="s">
         <v>109</v>
       </c>
@@ -4679,7 +4692,7 @@
         <v>3.9606970497928336E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="100" t="s">
         <v>152</v>
       </c>
@@ -4728,7 +4741,7 @@
       </c>
       <c r="Q35" s="27"/>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A36" s="100"/>
       <c r="B36">
         <v>1</v>
@@ -4770,7 +4783,7 @@
       <c r="P36" s="33"/>
       <c r="Q36" s="1"/>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="O37" s="30" t="s">
         <v>132</v>
       </c>
@@ -4779,7 +4792,7 @@
         <v>0.36558472469589065</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="O38" s="30" t="s">
         <v>133</v>
       </c>
@@ -4788,7 +4801,7 @@
         <v>0.14493952061648674</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="O39" s="30" t="s">
         <v>110</v>
       </c>
@@ -4797,7 +4810,7 @@
         <v>0.36558472469589065</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="O40" s="30" t="s">
         <v>111</v>
       </c>
@@ -4806,7 +4819,7 @@
         <v>0.14493952061648674</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="O42" s="30" t="s">
         <v>128</v>
       </c>
@@ -4815,7 +4828,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="O43" s="30" t="s">
         <v>127</v>
       </c>
@@ -4824,7 +4837,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
       <c r="O44" s="30" t="s">
         <v>131</v>
       </c>
@@ -4852,24 +4865,24 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:BC44"/>
+  <dimension ref="A1:BE44"/>
   <sheetViews>
-    <sheetView topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AO5" sqref="AO5"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AM5" sqref="AM5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.85546875" customWidth="1"/>
-    <col min="35" max="35" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12" bestFit="1" customWidth="1"/>
-    <col min="46" max="47" width="12" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.88671875" customWidth="1"/>
+    <col min="35" max="35" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="12" bestFit="1" customWidth="1"/>
+    <col min="48" max="49" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A1" s="49" t="s">
         <v>112</v>
       </c>
@@ -4887,7 +4900,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:55" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:57" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="52" t="s">
         <v>112</v>
       </c>
@@ -4906,7 +4919,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="4" spans="1:55" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:57" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="98" t="s">
         <v>70</v>
       </c>
@@ -5019,59 +5032,65 @@
         <v>27</v>
       </c>
       <c r="AL4" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="AM4" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="AN4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AM4" s="5" t="s">
+      <c r="AO4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AN4" s="5" t="s">
+      <c r="AP4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AO4" s="96" t="s">
+      <c r="AQ4" s="96" t="s">
         <v>177</v>
       </c>
-      <c r="AP4" s="12" t="s">
+      <c r="AR4" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="AQ4" s="12" t="s">
+      <c r="AS4" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="AR4" s="12" t="s">
+      <c r="AT4" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="AS4" s="12" t="s">
+      <c r="AU4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AT4" s="12" t="s">
+      <c r="AV4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="AU4" s="12" t="s">
+      <c r="AW4" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="AV4" s="85" t="s">
+      <c r="AX4" s="85" t="s">
         <v>160</v>
       </c>
-      <c r="AW4" s="6" t="s">
+      <c r="AY4" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="AX4" s="6" t="s">
+      <c r="AZ4" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AY4" s="6" t="s">
+      <c r="BA4" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="AZ4" s="6" t="s">
+      <c r="BB4" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="BA4" s="6" t="s">
+      <c r="BC4" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="BB4" s="6"/>
-      <c r="BC4" s="6" t="s">
+      <c r="BD4" s="6"/>
+      <c r="BE4" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A5" s="98"/>
       <c r="B5">
         <v>1</v>
@@ -5166,100 +5185,105 @@
         <v>33</v>
       </c>
       <c r="AE5" s="1">
-        <f t="shared" ref="AE5:AE12" si="0">AK5*$AQ$15</f>
+        <f t="shared" ref="AE5:AE12" si="0">AK5*$AS$15</f>
         <v>9.0399389163552328</v>
       </c>
       <c r="AF5" s="1">
-        <f t="shared" ref="AF5:AF12" si="1">AK5*$AS5</f>
+        <f t="shared" ref="AF5:AF12" si="1">AK5*$AU5</f>
         <v>1.0111902874411887</v>
       </c>
       <c r="AG5" s="24">
-        <f t="shared" ref="AG5:AG12" si="2">AK5*$AV5</f>
+        <f t="shared" ref="AG5:AG12" si="2">AK5*$AX5</f>
         <v>9.0399389163552328</v>
       </c>
       <c r="AH5" s="28">
-        <f t="shared" ref="AH5:AH12" si="3">AK5*$AT5</f>
+        <f t="shared" ref="AH5:AH12" si="3">AK5*$AV5</f>
         <v>10.111902874411886</v>
       </c>
       <c r="AI5" s="1">
-        <f>AZ5</f>
+        <f>BB5</f>
         <v>2.0477283347659267E-3</v>
       </c>
       <c r="AJ5" s="1">
-        <f>BC5</f>
+        <f>BE5</f>
         <v>1.3244862745926676E-6</v>
       </c>
       <c r="AK5" s="1">
         <f>AI5+AJ5</f>
         <v>2.0490528210405194E-3</v>
       </c>
-      <c r="AL5" s="1">
+      <c r="AL5" s="102">
+        <f>BC5+AJ5</f>
+        <v>4.0290524251749369E-3</v>
+      </c>
+      <c r="AM5" s="1"/>
+      <c r="AN5" s="1">
         <f>AI5*0.005</f>
         <v>1.0238641673829634E-5</v>
       </c>
-      <c r="AM5">
+      <c r="AO5">
         <f>AJ5*0.005</f>
         <v>6.6224313729633385E-9</v>
       </c>
-      <c r="AN5">
-        <f>AL5+AM5</f>
+      <c r="AP5">
+        <f>AN5+AO5</f>
         <v>1.0245264105202596E-5</v>
       </c>
-      <c r="AO5" s="1">
+      <c r="AQ5" s="1">
         <v>1800</v>
       </c>
-      <c r="AP5" s="58">
-        <f t="shared" ref="AP5:AP12" si="4">AK5+AE5*$E$31+AF5*$F$31+AH5*$J$31</f>
+      <c r="AR5" s="58">
+        <f t="shared" ref="AR5:AR12" si="4">AK5+AE5*$E$31+AF5*$F$31+AH5*$J$31</f>
         <v>3.3497283868557494E-3</v>
       </c>
-      <c r="AQ5" s="59">
-        <f t="shared" ref="AQ5:AQ12" si="5">(1-AK5/AP5)*100</f>
+      <c r="AS5" s="59">
+        <f t="shared" ref="AS5:AS12" si="5">(1-AK5/AR5)*100</f>
         <v>38.829284515098252</v>
       </c>
-      <c r="AR5" s="13">
+      <c r="AT5" s="13">
         <v>4.5999999999999996</v>
       </c>
-      <c r="AS5" s="13">
-        <f t="shared" ref="AS5:AS12" si="6">(($AR5/100)*(1+($AQ$15+$AV5)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AR5/100))</f>
+      <c r="AU5" s="13">
+        <f t="shared" ref="AU5:AU12" si="6">(($AT5/100)*(1+($AS$15+$AX5)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AT5/100))</f>
         <v>493.49156696102204</v>
       </c>
-      <c r="AT5" s="13">
-        <f t="shared" ref="AT5:AT12" si="7">$AS5/$X$23</f>
+      <c r="AV5" s="13">
+        <f t="shared" ref="AV5:AV12" si="7">$AU5/$X$23</f>
         <v>4934.91566961022</v>
       </c>
-      <c r="AU5" s="13">
+      <c r="AW5" s="13">
         <v>10</v>
       </c>
-      <c r="AV5" s="71">
-        <f t="shared" ref="AV5:AV12" si="8">$AU5/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+      <c r="AX5" s="71">
+        <f t="shared" ref="AX5:AX12" si="8">$AW5/100/(1-$X$33)*$X$32*10^6/$X$30</f>
         <v>4411.7647058823532</v>
       </c>
-      <c r="AW5" s="7">
+      <c r="AY5" s="7">
         <v>851425</v>
       </c>
-      <c r="AX5" s="8">
+      <c r="AZ5" s="8">
         <f>$T$27+$T$28*$T$30*(J5)^$T$29</f>
         <v>9.1058115591388438E-4</v>
       </c>
-      <c r="AY5" s="7">
-        <f t="shared" ref="AY5:AY12" si="9">J5*Z5</f>
+      <c r="BA5" s="7">
+        <f t="shared" ref="BA5:BA12" si="9">J5*Z5</f>
         <v>2.6054999999999997E-3</v>
       </c>
-      <c r="AZ5" s="8">
-        <f>((AY5-AX5)/($T$31-AW5))*(F5-$T$31)+AY5</f>
+      <c r="BB5" s="8">
+        <f>((BA5-AZ5)/($T$31-AY5))*(F5-$T$31)+BA5</f>
         <v>2.0477283347659267E-3</v>
       </c>
-      <c r="BA5" s="8">
-        <f t="shared" ref="BA5:BA12" si="10">$T$27+$T$28*$T$30*(L5)^$T$29</f>
+      <c r="BC5" s="8">
+        <f t="shared" ref="BC5:BC12" si="10">$T$27+$T$28*$T$30*(L5)^$T$29</f>
         <v>4.0277279389003447E-3</v>
       </c>
-      <c r="BB5" s="7"/>
-      <c r="BC5" s="7">
-        <f t="shared" ref="BC5:BC12" si="11">$AX$20*$AW$22*$AW$24*(M5)^$AW$21</f>
+      <c r="BD5" s="7"/>
+      <c r="BE5" s="7">
+        <f t="shared" ref="BE5:BE12" si="11">$AZ$20*$AY$22*$AY$24*(M5)^$AY$21</f>
         <v>1.3244862745926676E-6</v>
       </c>
     </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A6" s="98"/>
       <c r="B6">
         <v>1</v>
@@ -5369,84 +5393,87 @@
         <v>6.5956141271581705</v>
       </c>
       <c r="AI6" s="1">
-        <f>BA6</f>
+        <f>BC6</f>
         <v>7.9355355356128927E-4</v>
       </c>
       <c r="AJ6" s="1">
-        <f>BC6</f>
+        <f>BE6</f>
         <v>1.6879744031468265E-7</v>
       </c>
-      <c r="AK6">
-        <f t="shared" ref="AK6:AK12" si="15">AI6+AJ6</f>
+      <c r="AK6" s="1">
+        <f>AI6+AJ6</f>
         <v>7.9372235100160394E-4</v>
       </c>
-      <c r="AL6">
-        <f t="shared" ref="AL6:AM12" si="16">AI6*0.005</f>
+      <c r="AM6" s="102" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN6">
+        <f>AI6*0.005</f>
         <v>3.9677677678064465E-6</v>
       </c>
-      <c r="AM6">
-        <f t="shared" si="16"/>
+      <c r="AO6">
+        <f>AJ6*0.005</f>
         <v>8.4398720157341326E-10</v>
       </c>
-      <c r="AN6">
-        <f t="shared" ref="AN6:AN12" si="17">AL6+AM6</f>
+      <c r="AP6">
+        <f t="shared" ref="AP6:AP12" si="15">AN6+AO6</f>
         <v>3.9686117550080197E-6</v>
       </c>
-      <c r="AO6" s="1">
+      <c r="AQ6" s="1">
         <v>1800</v>
       </c>
-      <c r="AP6" s="58">
+      <c r="AR6" s="58">
         <f t="shared" si="4"/>
         <v>1.5736842407450208E-3</v>
       </c>
-      <c r="AQ6" s="59">
+      <c r="AS6" s="59">
         <f t="shared" si="5"/>
         <v>49.562794717583479</v>
       </c>
-      <c r="AR6" s="13">
+      <c r="AT6" s="13">
         <v>6.5</v>
       </c>
-      <c r="AS6" s="13">
+      <c r="AU6" s="13">
         <f t="shared" si="6"/>
         <v>830.97245766546928</v>
       </c>
-      <c r="AT6" s="13">
+      <c r="AV6" s="13">
         <f t="shared" si="7"/>
         <v>8309.724576654693</v>
       </c>
-      <c r="AU6" s="13">
+      <c r="AW6" s="13">
         <v>5</v>
       </c>
-      <c r="AV6" s="71">
+      <c r="AX6" s="71">
         <f t="shared" si="8"/>
         <v>2205.8823529411766</v>
       </c>
-      <c r="AW6" s="7">
+      <c r="AY6" s="7">
         <v>818263</v>
       </c>
-      <c r="AX6" s="8">
+      <c r="AZ6" s="8">
         <f>$T$27+$T$28*$T$30*(J6)^$T$29</f>
         <v>9.1017858127080242E-4</v>
       </c>
-      <c r="AY6" s="7" t="e">
+      <c r="BA6" s="7" t="e">
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AZ6" s="8" t="e">
-        <f>((AY6-AX6)/($T$31-AW6))*(F6-$T$31)+AY6</f>
+      <c r="BB6" s="8" t="e">
+        <f>((BA6-AZ6)/($T$31-AY6))*(F6-$T$31)+BA6</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BA6" s="8">
+      <c r="BC6" s="8">
         <f t="shared" si="10"/>
         <v>7.9355355356128927E-4</v>
       </c>
-      <c r="BB6" s="7"/>
-      <c r="BC6" s="7">
+      <c r="BD6" s="7"/>
+      <c r="BE6" s="7">
         <f t="shared" si="11"/>
         <v>1.6879744031468265E-7</v>
       </c>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A7" s="98"/>
       <c r="B7">
         <v>1</v>
@@ -5556,81 +5583,84 @@
         <v>0.54184269937105289</v>
       </c>
       <c r="AI7" s="1">
-        <f>BA7</f>
+        <f>BC7</f>
         <v>2.9792072957780891E-5</v>
       </c>
       <c r="AJ7" s="1">
         <v>0</v>
       </c>
       <c r="AK7">
+        <f t="shared" ref="AK6:AK12" si="16">AI7+AJ7</f>
+        <v>2.9792072957780891E-5</v>
+      </c>
+      <c r="AM7" s="102" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN7">
+        <f>AI7*0.005</f>
+        <v>1.4896036478890447E-7</v>
+      </c>
+      <c r="AO7">
+        <f>AJ7*0.005</f>
+        <v>0</v>
+      </c>
+      <c r="AP7">
         <f t="shared" si="15"/>
-        <v>2.9792072957780891E-5</v>
-      </c>
-      <c r="AL7">
-        <f t="shared" si="16"/>
         <v>1.4896036478890447E-7</v>
       </c>
-      <c r="AM7">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AN7">
-        <f t="shared" si="17"/>
-        <v>1.4896036478890447E-7</v>
-      </c>
-      <c r="AO7" s="1">
+      <c r="AQ7" s="1">
         <v>1800</v>
       </c>
-      <c r="AP7" s="58">
+      <c r="AR7" s="58">
         <f t="shared" si="4"/>
         <v>8.9403557211611783E-5</v>
       </c>
-      <c r="AQ7" s="59">
+      <c r="AS7" s="59">
         <f t="shared" si="5"/>
         <v>66.676859526668281</v>
       </c>
-      <c r="AR7" s="13">
+      <c r="AT7" s="13">
         <v>9.5</v>
       </c>
-      <c r="AS7" s="13">
+      <c r="AU7" s="13">
         <f t="shared" si="6"/>
         <v>1818.7478935719314</v>
       </c>
-      <c r="AT7" s="13">
+      <c r="AV7" s="13">
         <f t="shared" si="7"/>
         <v>18187.478935719311</v>
       </c>
-      <c r="AU7" s="13">
-        <v>0</v>
-      </c>
-      <c r="AV7" s="71">
+      <c r="AW7" s="13">
+        <v>0</v>
+      </c>
+      <c r="AX7" s="71">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AW7" s="7"/>
-      <c r="AX7" s="8" t="e">
-        <f t="shared" ref="AX7:AX12" si="18">$T$27+$T$28*$T$30*(T7*$T$32)^$T$29</f>
+      <c r="AY7" s="7"/>
+      <c r="AZ7" s="8" t="e">
+        <f t="shared" ref="AZ7:AZ12" si="17">$T$27+$T$28*$T$30*(T7*$T$32)^$T$29</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AY7" s="7" t="e">
+      <c r="BA7" s="7" t="e">
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AZ7" s="8" t="e">
-        <f t="shared" ref="AZ7:AZ12" si="19">AX7+((AY7-AX7)/$T$31)*F7</f>
+      <c r="BB7" s="8" t="e">
+        <f t="shared" ref="BB7:BB12" si="18">AZ7+((BA7-AZ7)/$T$31)*F7</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BA7" s="8">
+      <c r="BC7" s="8">
         <f t="shared" si="10"/>
         <v>2.9792072957780891E-5</v>
       </c>
-      <c r="BB7" s="7"/>
-      <c r="BC7" s="7">
+      <c r="BD7" s="7"/>
+      <c r="BE7" s="7">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A8" s="98"/>
       <c r="B8">
         <v>1</v>
@@ -5658,7 +5688,7 @@
         <v>33</v>
       </c>
       <c r="J8">
-        <f t="shared" ref="J8:J12" si="20">J7-M8</f>
+        <f t="shared" ref="J8:J12" si="19">J7-M8</f>
         <v>2.894E-2</v>
       </c>
       <c r="K8" s="38">
@@ -5740,81 +5770,84 @@
         <v>0.14688630816538931</v>
       </c>
       <c r="AI8" s="1">
-        <f t="shared" ref="AI8:AI12" si="21">BA8</f>
+        <f t="shared" ref="AI8:AI12" si="20">BC8</f>
         <v>8.076232483046996E-6</v>
       </c>
       <c r="AJ8" s="1">
         <v>0</v>
       </c>
       <c r="AK8">
+        <f t="shared" si="16"/>
+        <v>8.076232483046996E-6</v>
+      </c>
+      <c r="AM8" s="102" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN8">
+        <f>AI8*0.005</f>
+        <v>4.0381162415234981E-8</v>
+      </c>
+      <c r="AO8">
+        <f>AJ8*0.005</f>
+        <v>0</v>
+      </c>
+      <c r="AP8">
         <f t="shared" si="15"/>
-        <v>8.076232483046996E-6</v>
-      </c>
-      <c r="AL8">
-        <f t="shared" si="16"/>
         <v>4.0381162415234981E-8</v>
       </c>
-      <c r="AM8">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AN8">
-        <f t="shared" si="17"/>
-        <v>4.0381162415234981E-8</v>
-      </c>
-      <c r="AO8" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP8" s="58">
+      <c r="AQ8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AR8" s="58">
         <f t="shared" si="4"/>
         <v>2.4236108506970847E-5</v>
       </c>
-      <c r="AQ8" s="59">
+      <c r="AS8" s="59">
         <f t="shared" si="5"/>
         <v>66.676859526668281</v>
       </c>
-      <c r="AR8" s="13">
+      <c r="AT8" s="13">
         <v>9.5</v>
       </c>
-      <c r="AS8" s="13">
+      <c r="AU8" s="13">
         <f t="shared" si="6"/>
         <v>1818.7478935719314</v>
       </c>
-      <c r="AT8" s="13">
+      <c r="AV8" s="13">
         <f t="shared" si="7"/>
         <v>18187.478935719311</v>
       </c>
-      <c r="AU8" s="13">
-        <v>0</v>
-      </c>
-      <c r="AV8" s="71">
+      <c r="AW8" s="13">
+        <v>0</v>
+      </c>
+      <c r="AX8" s="71">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AW8" s="7"/>
-      <c r="AX8" s="8" t="e">
+      <c r="AY8" s="7"/>
+      <c r="AZ8" s="8" t="e">
+        <f t="shared" si="17"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA8" s="7" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB8" s="8" t="e">
         <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AY8" s="7" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ8" s="8" t="e">
-        <f t="shared" si="19"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA8" s="8">
+      <c r="BC8" s="8">
         <f t="shared" si="10"/>
         <v>8.076232483046996E-6</v>
       </c>
-      <c r="BB8" s="7"/>
-      <c r="BC8" s="7">
+      <c r="BD8" s="7"/>
+      <c r="BE8" s="7">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A9" s="98"/>
       <c r="B9">
         <v>1</v>
@@ -5842,7 +5875,7 @@
         <v>33</v>
       </c>
       <c r="J9">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.894E-2</v>
       </c>
       <c r="K9" s="38">
@@ -5924,81 +5957,84 @@
         <v>5.026843693451561E-2</v>
       </c>
       <c r="AI9" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>2.7639035136305163E-6</v>
       </c>
       <c r="AJ9" s="1">
         <v>0</v>
       </c>
       <c r="AK9">
+        <f t="shared" si="16"/>
+        <v>2.7639035136305163E-6</v>
+      </c>
+      <c r="AM9" s="102" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN9">
+        <f>AI9*0.005</f>
+        <v>1.3819517568152583E-8</v>
+      </c>
+      <c r="AO9">
+        <f>AJ9*0.005</f>
+        <v>0</v>
+      </c>
+      <c r="AP9">
         <f t="shared" si="15"/>
-        <v>2.7639035136305163E-6</v>
-      </c>
-      <c r="AL9">
-        <f t="shared" si="16"/>
         <v>1.3819517568152583E-8</v>
       </c>
-      <c r="AM9">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AN9">
-        <f t="shared" si="17"/>
-        <v>1.3819517568152583E-8</v>
-      </c>
-      <c r="AO9" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP9" s="58">
+      <c r="AQ9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AR9" s="58">
         <f t="shared" si="4"/>
         <v>8.294246803786242E-6</v>
       </c>
-      <c r="AQ9" s="59">
+      <c r="AS9" s="59">
         <f t="shared" si="5"/>
         <v>66.676859526668281</v>
       </c>
-      <c r="AR9" s="13">
+      <c r="AT9" s="13">
         <v>9.5</v>
       </c>
-      <c r="AS9" s="13">
+      <c r="AU9" s="13">
         <f t="shared" si="6"/>
         <v>1818.7478935719314</v>
       </c>
-      <c r="AT9" s="13">
+      <c r="AV9" s="13">
         <f t="shared" si="7"/>
         <v>18187.478935719311</v>
       </c>
-      <c r="AU9" s="13">
-        <v>0</v>
-      </c>
-      <c r="AV9" s="71">
+      <c r="AW9" s="13">
+        <v>0</v>
+      </c>
+      <c r="AX9" s="71">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AW9" s="7"/>
-      <c r="AX9" s="8" t="e">
+      <c r="AY9" s="7"/>
+      <c r="AZ9" s="8" t="e">
+        <f t="shared" si="17"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA9" s="7" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB9" s="8" t="e">
         <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AY9" s="7" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ9" s="8" t="e">
-        <f t="shared" si="19"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA9" s="8">
+      <c r="BC9" s="8">
         <f t="shared" si="10"/>
         <v>2.7639035136305163E-6</v>
       </c>
-      <c r="BB9" s="7"/>
-      <c r="BC9" s="7">
+      <c r="BD9" s="7"/>
+      <c r="BE9" s="7">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A10" s="98"/>
       <c r="B10">
         <v>1</v>
@@ -6026,7 +6062,7 @@
         <v>33</v>
       </c>
       <c r="J10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.894E-2</v>
       </c>
       <c r="K10" s="38">
@@ -6108,81 +6144,84 @@
         <v>2.1834134006527964E-2</v>
       </c>
       <c r="AI10" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>1.2005036038088161E-6</v>
       </c>
       <c r="AJ10" s="1">
         <v>0</v>
       </c>
       <c r="AK10">
+        <f t="shared" si="16"/>
+        <v>1.2005036038088161E-6</v>
+      </c>
+      <c r="AM10" s="102" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN10">
+        <f>AI10*0.005</f>
+        <v>6.0025180190440811E-9</v>
+      </c>
+      <c r="AO10">
+        <f>AJ10*0.005</f>
+        <v>0</v>
+      </c>
+      <c r="AP10">
         <f t="shared" si="15"/>
-        <v>1.2005036038088161E-6</v>
-      </c>
-      <c r="AL10">
-        <f t="shared" si="16"/>
         <v>6.0025180190440811E-9</v>
       </c>
-      <c r="AM10">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AN10">
-        <f t="shared" si="17"/>
-        <v>6.0025180190440811E-9</v>
-      </c>
-      <c r="AO10" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP10" s="58">
+      <c r="AQ10" t="s">
+        <v>32</v>
+      </c>
+      <c r="AR10" s="58">
         <f t="shared" si="4"/>
         <v>3.6026124391534188E-6</v>
       </c>
-      <c r="AQ10" s="59">
+      <c r="AS10" s="59">
         <f t="shared" si="5"/>
         <v>66.676859526668281</v>
       </c>
-      <c r="AR10" s="13">
+      <c r="AT10" s="13">
         <v>9.5</v>
       </c>
-      <c r="AS10" s="13">
+      <c r="AU10" s="13">
         <f t="shared" si="6"/>
         <v>1818.7478935719314</v>
       </c>
-      <c r="AT10" s="13">
+      <c r="AV10" s="13">
         <f t="shared" si="7"/>
         <v>18187.478935719311</v>
       </c>
-      <c r="AU10" s="13">
-        <v>0</v>
-      </c>
-      <c r="AV10" s="71">
+      <c r="AW10" s="13">
+        <v>0</v>
+      </c>
+      <c r="AX10" s="71">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AW10" s="7"/>
-      <c r="AX10" s="8" t="e">
+      <c r="AY10" s="7"/>
+      <c r="AZ10" s="8" t="e">
+        <f t="shared" si="17"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA10" s="7" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB10" s="8" t="e">
         <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AY10" s="7" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ10" s="8" t="e">
-        <f t="shared" si="19"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA10" s="8">
+      <c r="BC10" s="8">
         <f t="shared" si="10"/>
         <v>1.2005036038088161E-6</v>
       </c>
-      <c r="BB10" s="7"/>
-      <c r="BC10" s="7">
+      <c r="BD10" s="7"/>
+      <c r="BE10" s="7">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A11" s="98"/>
       <c r="B11">
         <v>1</v>
@@ -6210,7 +6249,7 @@
         <v>33</v>
       </c>
       <c r="J11">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.894E-2</v>
       </c>
       <c r="K11" s="38">
@@ -6292,81 +6331,84 @@
         <v>7.8932588657893536E-3</v>
       </c>
       <c r="AI11" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>4.3399411725433714E-7</v>
       </c>
       <c r="AJ11" s="1">
         <v>0</v>
       </c>
       <c r="AK11">
+        <f t="shared" si="16"/>
+        <v>4.3399411725433714E-7</v>
+      </c>
+      <c r="AM11" s="102" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN11">
+        <f>AI11*0.005</f>
+        <v>2.1699705862716857E-9</v>
+      </c>
+      <c r="AO11">
+        <f>AJ11*0.005</f>
+        <v>0</v>
+      </c>
+      <c r="AP11">
         <f t="shared" si="15"/>
-        <v>4.3399411725433714E-7</v>
-      </c>
-      <c r="AL11">
-        <f t="shared" si="16"/>
         <v>2.1699705862716857E-9</v>
       </c>
-      <c r="AM11">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AN11">
-        <f t="shared" si="17"/>
-        <v>2.1699705862716857E-9</v>
-      </c>
-      <c r="AO11" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP11" s="58">
+      <c r="AQ11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AR11" s="58">
         <f t="shared" si="4"/>
         <v>1.3023806012571343E-6</v>
       </c>
-      <c r="AQ11" s="59">
+      <c r="AS11" s="59">
         <f t="shared" si="5"/>
         <v>66.676859526668281</v>
       </c>
-      <c r="AR11" s="13">
+      <c r="AT11" s="13">
         <v>9.5</v>
       </c>
-      <c r="AS11" s="13">
+      <c r="AU11" s="13">
         <f t="shared" si="6"/>
         <v>1818.7478935719314</v>
       </c>
-      <c r="AT11" s="13">
+      <c r="AV11" s="13">
         <f t="shared" si="7"/>
         <v>18187.478935719311</v>
       </c>
-      <c r="AU11" s="13">
-        <v>0</v>
-      </c>
-      <c r="AV11" s="71">
+      <c r="AW11" s="13">
+        <v>0</v>
+      </c>
+      <c r="AX11" s="71">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AW11" s="7"/>
-      <c r="AX11" s="8" t="e">
+      <c r="AY11" s="7"/>
+      <c r="AZ11" s="8" t="e">
+        <f t="shared" si="17"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA11" s="7" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB11" s="8" t="e">
         <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AY11" s="7" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ11" s="8" t="e">
-        <f t="shared" si="19"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA11" s="8">
+      <c r="BC11" s="8">
         <f t="shared" si="10"/>
         <v>4.3399411725433714E-7</v>
       </c>
-      <c r="BB11" s="7"/>
-      <c r="BC11" s="7">
+      <c r="BD11" s="7"/>
+      <c r="BE11" s="7">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A12" s="98"/>
       <c r="B12">
         <v>1</v>
@@ -6394,7 +6436,7 @@
         <v>33</v>
       </c>
       <c r="J12">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.894E-2</v>
       </c>
       <c r="K12" s="38">
@@ -6476,81 +6518,84 @@
         <v>5.2997814357572583E-3</v>
       </c>
       <c r="AI12" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>2.9139725491853351E-7</v>
       </c>
       <c r="AJ12" s="1">
         <v>0</v>
       </c>
       <c r="AK12">
+        <f t="shared" si="16"/>
+        <v>2.9139725491853351E-7</v>
+      </c>
+      <c r="AM12" s="102" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN12">
+        <f>AI12*0.005</f>
+        <v>1.4569862745926675E-9</v>
+      </c>
+      <c r="AO12">
+        <f>AJ12*0.005</f>
+        <v>0</v>
+      </c>
+      <c r="AP12">
         <f t="shared" si="15"/>
-        <v>2.9139725491853351E-7</v>
-      </c>
-      <c r="AL12">
-        <f t="shared" si="16"/>
         <v>1.4569862745926675E-9</v>
       </c>
-      <c r="AM12">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AN12">
-        <f t="shared" si="17"/>
-        <v>1.4569862745926675E-9</v>
-      </c>
-      <c r="AO12" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP12" s="61">
+      <c r="AQ12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AR12" s="61">
         <f t="shared" si="4"/>
         <v>8.7445916195004701E-7</v>
       </c>
-      <c r="AQ12" s="60">
+      <c r="AS12" s="60">
         <f t="shared" si="5"/>
         <v>66.676859526668281</v>
       </c>
-      <c r="AR12" s="14">
+      <c r="AT12" s="14">
         <v>9.5</v>
       </c>
-      <c r="AS12" s="13">
+      <c r="AU12" s="13">
         <f t="shared" si="6"/>
         <v>1818.7478935719314</v>
       </c>
-      <c r="AT12" s="14">
+      <c r="AV12" s="14">
         <f t="shared" si="7"/>
         <v>18187.478935719311</v>
       </c>
-      <c r="AU12" s="14">
-        <v>0</v>
-      </c>
-      <c r="AV12" s="71">
+      <c r="AW12" s="14">
+        <v>0</v>
+      </c>
+      <c r="AX12" s="71">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AW12" s="7"/>
-      <c r="AX12" s="8" t="e">
+      <c r="AY12" s="7"/>
+      <c r="AZ12" s="8" t="e">
+        <f t="shared" si="17"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA12" s="7" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB12" s="8" t="e">
         <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AY12" s="7" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ12" s="8" t="e">
-        <f t="shared" si="19"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA12" s="8">
+      <c r="BC12" s="8">
         <f t="shared" si="10"/>
         <v>2.9139725491853351E-7</v>
       </c>
-      <c r="BB12" s="7"/>
-      <c r="BC12" s="7">
+      <c r="BD12" s="7"/>
+      <c r="BE12" s="7">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
@@ -6562,7 +6607,7 @@
       <c r="AE13" s="1"/>
       <c r="AF13" s="1"/>
     </row>
-    <row r="14" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="98" t="s">
         <v>71</v>
       </c>
@@ -6650,20 +6695,20 @@
       </c>
       <c r="AF14" s="3"/>
       <c r="AG14" s="3"/>
-      <c r="AP14" s="22"/>
-      <c r="AQ14" s="67" t="s">
+      <c r="AR14" s="22"/>
+      <c r="AS14" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="AR14" s="67" t="s">
+      <c r="AT14" s="67" t="s">
         <v>135</v>
       </c>
-      <c r="AS14" s="68" t="s">
+      <c r="AU14" s="68" t="s">
         <v>115</v>
       </c>
-      <c r="AT14" s="40"/>
-      <c r="AU14" s="40"/>
-    </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AV14" s="40"/>
+      <c r="AW14" s="40"/>
+    </row>
+    <row r="15" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A15" s="98"/>
       <c r="B15">
         <v>1</v>
@@ -6703,15 +6748,15 @@
         <v>1.6239747221660625</v>
       </c>
       <c r="M15">
-        <f t="shared" ref="M15:M20" si="22">J15*$X15</f>
+        <f t="shared" ref="M15:M20" si="21">J15*$X15</f>
         <v>16.239747221660625</v>
       </c>
       <c r="N15">
-        <f t="shared" ref="N15:N20" si="23">AA15*$J15</f>
+        <f t="shared" ref="N15:N20" si="22">AA15*$J15</f>
         <v>0</v>
       </c>
       <c r="O15" s="1">
-        <f t="shared" ref="O15:O20" si="24">J15*$AB$16</f>
+        <f t="shared" ref="O15:O20" si="23">J15*$AB$16</f>
         <v>18.09675</v>
       </c>
       <c r="P15">
@@ -6737,7 +6782,7 @@
         <v>4.3</v>
       </c>
       <c r="W15" s="13">
-        <f t="shared" ref="W15:W20" si="25">(($V15/100)*(1+$AB$16*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$V15/100))</f>
+        <f t="shared" ref="W15:W20" si="24">(($V15/100)*(1+$AB$16*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$V15/100))</f>
         <v>395.90503059926971</v>
       </c>
       <c r="X15" s="13">
@@ -6751,14 +6796,14 @@
         <v>27</v>
       </c>
       <c r="AA15" s="76">
-        <f t="shared" ref="AA15:AA20" si="26">IF(F15="HiddenElement",$AA$22/100/(1-$X$33)*$X$32*10^6/$X$30,0)</f>
+        <f t="shared" ref="AA15:AA20" si="25">IF(F15="HiddenElement",$AA$22/100/(1-$X$33)*$X$32*10^6/$X$30,0)</f>
         <v>0</v>
       </c>
       <c r="AB15" s="75" t="s">
         <v>21</v>
       </c>
       <c r="AC15" s="13">
-        <f>ROUND(X15/$AT$6*120,0)</f>
+        <f>ROUND(X15/$AV$6*120,0)</f>
         <v>57</v>
       </c>
       <c r="AD15" s="13">
@@ -6770,23 +6815,23 @@
         <v>34.818239239744116</v>
       </c>
       <c r="AF15" s="1"/>
-      <c r="AP15" s="69"/>
-      <c r="AQ15" s="71">
-        <f>$AQ$16/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+      <c r="AR15" s="69"/>
+      <c r="AS15" s="71">
+        <f>$AS$16/100/(1-$X$33)*$X$32*10^6/$X$30</f>
         <v>4411.7647058823532</v>
       </c>
-      <c r="AR15" s="71">
-        <f>$AR$16/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+      <c r="AT15" s="71">
+        <f>$AT$16/100/(1-$X$33)*$X$32*10^6/$X$30</f>
         <v>4411.7647058823532</v>
       </c>
-      <c r="AS15" s="72">
-        <f>AR15+AQ15</f>
+      <c r="AU15" s="72">
+        <f>AT15+AS15</f>
         <v>8823.5294117647063</v>
       </c>
-      <c r="AT15" s="83"/>
-      <c r="AU15" s="83"/>
-    </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AV15" s="83"/>
+      <c r="AW15" s="83"/>
+    </row>
+    <row r="16" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A16" s="98"/>
       <c r="B16">
         <v>1</v>
@@ -6818,7 +6863,7 @@
         <v>1.7099999999999999E-3</v>
       </c>
       <c r="K16">
-        <f t="shared" ref="K16:K20" si="27">J16*0.005</f>
+        <f t="shared" ref="K16:K20" si="26">J16*0.005</f>
         <v>8.5499999999999995E-6</v>
       </c>
       <c r="L16">
@@ -6826,22 +6871,22 @@
         <v>0.19277131424832977</v>
       </c>
       <c r="M16">
+        <f t="shared" si="21"/>
+        <v>1.9277131424832974</v>
+      </c>
+      <c r="N16">
         <f t="shared" si="22"/>
-        <v>1.9277131424832974</v>
-      </c>
-      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="O16" s="1">
-        <f t="shared" si="24"/>
         <v>7.5441176470588234</v>
       </c>
       <c r="P16">
         <v>2.6861000000000002E-4</v>
       </c>
       <c r="Q16" s="1">
-        <f t="shared" ref="Q16:Q20" si="28">J16*$AC16</f>
+        <f t="shared" ref="Q16:Q20" si="27">J16*$AC16</f>
         <v>2.7359999999999999E-2</v>
       </c>
       <c r="R16">
@@ -6861,7 +6906,7 @@
         <v>1.8</v>
       </c>
       <c r="W16" s="13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>112.73176271832151</v>
       </c>
       <c r="X16" s="13">
@@ -6875,7 +6920,7 @@
         <v>1</v>
       </c>
       <c r="AA16" s="76">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="AB16" s="45">
@@ -6883,35 +6928,35 @@
         <v>4411.7647058823532</v>
       </c>
       <c r="AC16" s="13">
-        <f t="shared" ref="AC16:AC20" si="29">ROUND(X16/$AT$6*120,0)</f>
+        <f t="shared" ref="AC16:AC20" si="28">ROUND(X16/$AV$6*120,0)</f>
         <v>16</v>
       </c>
       <c r="AD16" s="13">
-        <f t="shared" ref="AD16:AD20" si="30">J16+L16*$F$31+M16*$J$31+O16*$E$31</f>
+        <f t="shared" ref="AD16:AD20" si="29">J16+L16*$F$31+M16*$J$31+O16*$E$31</f>
         <v>2.1242656885690431E-3</v>
       </c>
       <c r="AE16" s="59">
-        <f t="shared" ref="AE16:AE20" si="31">(1-J16/AD16)*100</f>
+        <f t="shared" ref="AE16:AE20" si="30">(1-J16/AD16)*100</f>
         <v>19.501594871030591</v>
       </c>
       <c r="AF16" s="1"/>
-      <c r="AP16" s="70" t="s">
+      <c r="AR16" s="70" t="s">
         <v>136</v>
       </c>
-      <c r="AQ16" s="73">
+      <c r="AS16" s="73">
         <v>10</v>
       </c>
-      <c r="AR16" s="73">
+      <c r="AT16" s="73">
         <v>10</v>
       </c>
-      <c r="AS16" s="74">
-        <f>AR16+AQ16</f>
+      <c r="AU16" s="74">
+        <f>AT16+AS16</f>
         <v>20</v>
       </c>
-      <c r="AT16" s="84"/>
-      <c r="AU16" s="84"/>
-    </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AV16" s="84"/>
+      <c r="AW16" s="84"/>
+    </row>
+    <row r="17" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A17" s="98"/>
       <c r="B17">
         <v>1</v>
@@ -6943,23 +6988,23 @@
         <v>5.0624699999999995E-3</v>
       </c>
       <c r="K17">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>2.5312349999999998E-5</v>
       </c>
       <c r="L17">
-        <f t="shared" ref="L17:L20" si="32">J17*$W17</f>
+        <f t="shared" ref="L17:L20" si="31">J17*$W17</f>
         <v>2.3758024102824513</v>
       </c>
       <c r="M17">
+        <f t="shared" si="21"/>
+        <v>23.758024102824514</v>
+      </c>
+      <c r="N17">
         <f t="shared" si="22"/>
-        <v>23.758024102824514</v>
-      </c>
-      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17" s="1">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="1">
-        <f t="shared" si="24"/>
         <v>22.334426470588234</v>
       </c>
       <c r="P17">
@@ -6985,37 +7030,37 @@
         <v>4.8</v>
       </c>
       <c r="W17" s="13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>469.29708428542818</v>
       </c>
       <c r="X17" s="13">
-        <f t="shared" ref="X17:X20" si="33">$W17/$X$23</f>
+        <f t="shared" ref="X17:X20" si="32">$W17/$X$23</f>
         <v>4692.9708428542817</v>
       </c>
       <c r="Z17" s="24"/>
       <c r="AA17" s="76">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="AB17" s="42">
         <v>10</v>
       </c>
       <c r="AC17" s="13">
+        <f t="shared" si="28"/>
+        <v>68</v>
+      </c>
+      <c r="AD17" s="13">
         <f t="shared" si="29"/>
-        <v>68</v>
-      </c>
-      <c r="AD17" s="13">
+        <v>8.1497066913228666E-3</v>
+      </c>
+      <c r="AE17" s="59">
         <f t="shared" si="30"/>
-        <v>8.1497066913228666E-3</v>
-      </c>
-      <c r="AE17" s="59">
-        <f t="shared" si="31"/>
         <v>37.88156811348685</v>
       </c>
       <c r="AF17" s="1"/>
       <c r="AG17" s="1"/>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A18" s="98"/>
       <c r="B18">
         <v>1</v>
@@ -7047,30 +7092,30 @@
         <v>2.2800000000000003E-3</v>
       </c>
       <c r="K18">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>1.1400000000000003E-5</v>
       </c>
       <c r="L18">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>0.36572238936056839</v>
       </c>
       <c r="M18">
+        <f t="shared" si="21"/>
+        <v>3.6572238936056838</v>
+      </c>
+      <c r="N18">
         <f t="shared" si="22"/>
-        <v>3.6572238936056838</v>
-      </c>
-      <c r="N18">
+        <v>3.0176470588235293</v>
+      </c>
+      <c r="O18" s="1">
         <f t="shared" si="23"/>
-        <v>3.0176470588235293</v>
-      </c>
-      <c r="O18" s="1">
-        <f t="shared" si="24"/>
         <v>10.058823529411766</v>
       </c>
       <c r="P18">
         <v>2.4800000000000001E-4</v>
       </c>
       <c r="Q18" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>5.2440000000000007E-2</v>
       </c>
       <c r="R18">
@@ -7090,11 +7135,11 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="W18" s="13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>160.40455673709138</v>
       </c>
       <c r="X18" s="13">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>1604.0455673709137</v>
       </c>
       <c r="AA18" s="76">
@@ -7105,21 +7150,21 @@
         <v>120</v>
       </c>
       <c r="AC18" s="13">
+        <f t="shared" si="28"/>
+        <v>23</v>
+      </c>
+      <c r="AD18" s="13">
         <f t="shared" si="29"/>
-        <v>23</v>
-      </c>
-      <c r="AD18" s="13">
+        <v>2.9444020852838065E-3</v>
+      </c>
+      <c r="AE18" s="59">
         <f t="shared" si="30"/>
-        <v>2.9444020852838065E-3</v>
-      </c>
-      <c r="AE18" s="59">
-        <f t="shared" si="31"/>
         <v>22.564923744773314</v>
       </c>
       <c r="AF18" s="1"/>
       <c r="AG18" s="1"/>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A19" s="98"/>
       <c r="B19">
         <v>1</v>
@@ -7151,30 +7196,30 @@
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="K19">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>2.0000000000000002E-7</v>
       </c>
       <c r="L19">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>6.4161822694836562E-3</v>
       </c>
       <c r="M19">
+        <f t="shared" si="21"/>
+        <v>6.4161822694836557E-2</v>
+      </c>
+      <c r="N19">
         <f t="shared" si="22"/>
-        <v>6.4161822694836557E-2</v>
-      </c>
-      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19" s="1">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="O19" s="1">
-        <f t="shared" si="24"/>
         <v>0.17647058823529413</v>
       </c>
       <c r="P19">
         <v>4.7099999999999998E-6</v>
       </c>
       <c r="Q19" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>9.2000000000000003E-4</v>
       </c>
       <c r="R19">
@@ -7194,41 +7239,41 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="W19" s="13">
+        <f t="shared" si="24"/>
+        <v>160.40455673709138</v>
+      </c>
+      <c r="X19" s="13">
+        <f t="shared" si="32"/>
+        <v>1604.0455673709137</v>
+      </c>
+      <c r="AA19" s="76">
         <f t="shared" si="25"/>
-        <v>160.40455673709138</v>
-      </c>
-      <c r="X19" s="13">
-        <f t="shared" si="33"/>
-        <v>1604.0455673709137</v>
-      </c>
-      <c r="AA19" s="76">
-        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="AB19" s="1"/>
       <c r="AC19" s="13">
+        <f t="shared" si="28"/>
+        <v>23</v>
+      </c>
+      <c r="AD19" s="13">
         <f t="shared" si="29"/>
-        <v>23</v>
-      </c>
-      <c r="AD19" s="13">
+        <v>5.1656176934803615E-5</v>
+      </c>
+      <c r="AE19" s="59">
         <f t="shared" si="30"/>
-        <v>5.1656176934803615E-5</v>
-      </c>
-      <c r="AE19" s="59">
-        <f t="shared" si="31"/>
         <v>22.564923744773303</v>
       </c>
-      <c r="AV19" s="97" t="s">
+      <c r="AX19" s="97" t="s">
         <v>57</v>
       </c>
-      <c r="AW19" s="7" t="s">
+      <c r="AY19" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="AX19" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AZ19" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A20" s="98"/>
       <c r="B20">
         <v>1</v>
@@ -7259,30 +7304,30 @@
         <v>4.0322099999999996E-3</v>
       </c>
       <c r="K20">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>2.0161049999999999E-5</v>
       </c>
       <c r="L20">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>2.0843008232103681</v>
       </c>
       <c r="M20">
+        <f t="shared" si="21"/>
+        <v>20.843008232103678</v>
+      </c>
+      <c r="N20">
         <f t="shared" si="22"/>
-        <v>20.843008232103678</v>
-      </c>
-      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20" s="1">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="O20" s="1">
-        <f t="shared" si="24"/>
         <v>17.789161764705881</v>
       </c>
       <c r="P20">
         <v>1.9201E-4</v>
       </c>
       <c r="Q20" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>0.30241574999999998</v>
       </c>
       <c r="R20">
@@ -7301,59 +7346,59 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="W20" s="14">
+        <f t="shared" si="24"/>
+        <v>516.91276575633913</v>
+      </c>
+      <c r="X20" s="14">
+        <f t="shared" si="32"/>
+        <v>5169.127657563391</v>
+      </c>
+      <c r="AA20" s="77">
         <f t="shared" si="25"/>
-        <v>516.91276575633913</v>
-      </c>
-      <c r="X20" s="14">
-        <f t="shared" si="33"/>
-        <v>5169.127657563391</v>
-      </c>
-      <c r="AA20" s="77">
-        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="AC20" s="14">
+        <f t="shared" si="28"/>
+        <v>75</v>
+      </c>
+      <c r="AD20" s="14">
         <f t="shared" si="29"/>
-        <v>75</v>
-      </c>
-      <c r="AD20" s="14">
+        <v>6.689085819105817E-3</v>
+      </c>
+      <c r="AE20" s="60">
         <f t="shared" si="30"/>
-        <v>6.689085819105817E-3</v>
-      </c>
-      <c r="AE20" s="60">
-        <f t="shared" si="31"/>
         <v>39.719565437732463</v>
       </c>
-      <c r="AV20" s="97"/>
-      <c r="AW20" s="7" t="s">
+      <c r="AX20" s="97"/>
+      <c r="AY20" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="AX20" s="7">
+      <c r="AZ20" s="7">
         <v>0.106</v>
       </c>
     </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="V21" s="79"/>
       <c r="W21" s="15"/>
       <c r="X21" s="48"/>
       <c r="Z21" s="1"/>
-      <c r="AN21" s="97"/>
-      <c r="AO21" s="97"/>
       <c r="AP21" s="97"/>
       <c r="AQ21" s="97"/>
       <c r="AR21" s="97"/>
       <c r="AS21" s="97"/>
       <c r="AT21" s="97"/>
       <c r="AU21" s="97"/>
-      <c r="AV21" s="7" t="s">
+      <c r="AV21" s="97"/>
+      <c r="AW21" s="97"/>
+      <c r="AX21" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="AW21" s="7">
+      <c r="AY21" s="7">
         <v>1.28</v>
       </c>
     </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="V22" s="29"/>
       <c r="W22" s="80"/>
@@ -7366,69 +7411,69 @@
       <c r="AA22" s="42">
         <v>3</v>
       </c>
-      <c r="AN22" s="97"/>
-      <c r="AO22" s="97"/>
       <c r="AP22" s="97"/>
       <c r="AQ22" s="97"/>
       <c r="AR22" s="97"/>
       <c r="AS22" s="97"/>
       <c r="AT22" s="97"/>
       <c r="AU22" s="97"/>
-      <c r="AV22" s="7" t="s">
+      <c r="AV22" s="97"/>
+      <c r="AW22" s="97"/>
+      <c r="AX22" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="AW22" s="7">
+      <c r="AY22" s="7">
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="X23" s="14">
         <v>0.1</v>
       </c>
       <c r="Y23" s="62">
-        <f>(SUMPRODUCT(V15:V20,AD15:AD20)+SUMPRODUCT(AR5:AR12,AP5:AP12))/SUM(AD15:AD20,AP5:AP12)</f>
+        <f>(SUMPRODUCT(V15:V20,AD15:AD20)+SUMPRODUCT(AT5:AT12,AR5:AR12))/SUM(AD15:AD20,AR5:AR12)</f>
         <v>4.4039658411029281</v>
       </c>
       <c r="AA23" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="AN23" s="97"/>
-      <c r="AO23" s="97"/>
       <c r="AP23" s="97"/>
       <c r="AQ23" s="97"/>
       <c r="AR23" s="97"/>
       <c r="AS23" s="97"/>
       <c r="AT23" s="97"/>
       <c r="AU23" s="97"/>
-      <c r="AV23" s="7" t="s">
+      <c r="AV23" s="97"/>
+      <c r="AW23" s="97"/>
+      <c r="AX23" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="AW23" s="7">
+      <c r="AY23" s="7">
         <f>210*3600*24/12</f>
         <v>1512000</v>
       </c>
     </row>
-    <row r="24" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="AN24" s="7"/>
-      <c r="AO24" s="7"/>
       <c r="AP24" s="7"/>
       <c r="AQ24" s="7"/>
       <c r="AR24" s="7"/>
       <c r="AS24" s="7"/>
       <c r="AT24" s="7"/>
       <c r="AU24" s="7"/>
-      <c r="AV24" s="7" t="s">
+      <c r="AV24" s="7"/>
+      <c r="AW24" s="7"/>
+      <c r="AX24" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AW24" s="7">
+      <c r="AY24" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A25" s="98" t="s">
         <v>72</v>
       </c>
@@ -7468,23 +7513,23 @@
       <c r="M25" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="AM25" s="9"/>
-      <c r="AN25" s="9"/>
       <c r="AO25" s="9"/>
       <c r="AP25" s="9"/>
       <c r="AQ25" s="9"/>
       <c r="AR25" s="9"/>
-      <c r="AS25" s="7" t="s">
+      <c r="AS25" s="9"/>
+      <c r="AT25" s="9"/>
+      <c r="AU25" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AT25" s="7"/>
-      <c r="AU25" s="7"/>
-      <c r="AV25" s="7">
+      <c r="AV25" s="7"/>
+      <c r="AW25" s="7"/>
+      <c r="AX25" s="7">
         <f>1/59</f>
         <v>1.6949152542372881E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A26" s="98"/>
       <c r="B26">
         <v>1</v>
@@ -7522,18 +7567,18 @@
       <c r="M26" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="AM26" s="10"/>
-      <c r="AN26" s="10"/>
       <c r="AO26" s="10"/>
       <c r="AP26" s="10"/>
       <c r="AQ26" s="10"/>
       <c r="AR26" s="10"/>
-      <c r="AS26" s="7"/>
-      <c r="AT26" s="7"/>
+      <c r="AS26" s="10"/>
+      <c r="AT26" s="10"/>
       <c r="AU26" s="7"/>
       <c r="AV26" s="7"/>
-    </row>
-    <row r="27" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AW26" s="7"/>
+      <c r="AX26" s="7"/>
+    </row>
+    <row r="27" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A27" s="98"/>
       <c r="B27">
         <v>1</v>
@@ -7598,18 +7643,18 @@
       <c r="T27" s="8">
         <v>2.6499999999999999E-8</v>
       </c>
-      <c r="AM27" s="10"/>
-      <c r="AN27" s="10"/>
       <c r="AO27" s="10"/>
       <c r="AP27" s="10"/>
       <c r="AQ27" s="10"/>
       <c r="AR27" s="10"/>
-      <c r="AS27" s="7"/>
-      <c r="AT27" s="7"/>
+      <c r="AS27" s="10"/>
+      <c r="AT27" s="10"/>
       <c r="AU27" s="7"/>
       <c r="AV27" s="7"/>
-    </row>
-    <row r="28" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AW27" s="7"/>
+      <c r="AX27" s="7"/>
+    </row>
+    <row r="28" spans="1:52" x14ac:dyDescent="0.3">
       <c r="E28" s="46">
         <f>AB16</f>
         <v>4411.7647058823532</v>
@@ -7650,20 +7695,20 @@
       <c r="T28" s="7">
         <v>0.106</v>
       </c>
-      <c r="AM28" s="10" t="s">
+      <c r="AO28" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="AN28" s="10"/>
-      <c r="AO28" s="10"/>
       <c r="AP28" s="10"/>
       <c r="AQ28" s="10"/>
       <c r="AR28" s="10"/>
-      <c r="AS28" s="7"/>
-      <c r="AT28" s="7"/>
+      <c r="AS28" s="10"/>
+      <c r="AT28" s="10"/>
       <c r="AU28" s="7"/>
       <c r="AV28" s="7"/>
-    </row>
-    <row r="29" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AW28" s="7"/>
+      <c r="AX28" s="7"/>
+    </row>
+    <row r="29" spans="1:52" x14ac:dyDescent="0.3">
       <c r="F29" s="1"/>
       <c r="R29" s="99"/>
       <c r="S29" s="7" t="s">
@@ -7678,20 +7723,20 @@
       <c r="X29" s="41">
         <v>180</v>
       </c>
-      <c r="AM29" s="11" t="s">
+      <c r="AO29" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="AN29" s="11"/>
-      <c r="AO29" s="11"/>
       <c r="AP29" s="11"/>
       <c r="AQ29" s="11"/>
       <c r="AR29" s="11"/>
-      <c r="AS29" s="7"/>
-      <c r="AT29" s="7"/>
+      <c r="AS29" s="11"/>
+      <c r="AT29" s="11"/>
       <c r="AU29" s="7"/>
       <c r="AV29" s="7"/>
-    </row>
-    <row r="30" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AW29" s="7"/>
+      <c r="AX29" s="7"/>
+    </row>
+    <row r="30" spans="1:52" x14ac:dyDescent="0.3">
       <c r="D30" s="23" t="s">
         <v>78</v>
       </c>
@@ -7716,18 +7761,18 @@
       <c r="X30" s="41">
         <v>340</v>
       </c>
-      <c r="AM30" s="11"/>
-      <c r="AN30" s="11"/>
       <c r="AO30" s="11"/>
       <c r="AP30" s="11"/>
       <c r="AQ30" s="11"/>
       <c r="AR30" s="11"/>
-      <c r="AS30" s="7"/>
-      <c r="AT30" s="7"/>
+      <c r="AS30" s="11"/>
+      <c r="AT30" s="11"/>
       <c r="AU30" s="7"/>
       <c r="AV30" s="7"/>
-    </row>
-    <row r="31" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AW30" s="7"/>
+      <c r="AX30" s="7"/>
+    </row>
+    <row r="31" spans="1:52" x14ac:dyDescent="0.3">
       <c r="D31" s="20" t="s">
         <v>79</v>
       </c>
@@ -7761,20 +7806,20 @@
       <c r="X31" s="32">
         <v>12</v>
       </c>
-      <c r="AM31" s="10" t="s">
+      <c r="AO31" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="AN31" s="10"/>
-      <c r="AO31" s="10"/>
       <c r="AP31" s="10"/>
       <c r="AQ31" s="10"/>
       <c r="AR31" s="10"/>
-      <c r="AS31" s="7"/>
-      <c r="AT31" s="7"/>
+      <c r="AS31" s="10"/>
+      <c r="AT31" s="10"/>
       <c r="AU31" s="7"/>
       <c r="AV31" s="7"/>
-    </row>
-    <row r="32" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AW31" s="7"/>
+      <c r="AX31" s="7"/>
+    </row>
+    <row r="32" spans="1:52" x14ac:dyDescent="0.3">
       <c r="D32" s="20" t="s">
         <v>76</v>
       </c>
@@ -7808,7 +7853,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="O33" s="30" t="s">
         <v>108</v>
       </c>
@@ -7823,7 +7868,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
       <c r="O34" s="30" t="s">
         <v>109</v>
       </c>
@@ -7832,7 +7877,7 @@
         <v>3.9622291936427113E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="100" t="s">
         <v>152</v>
       </c>
@@ -7881,7 +7926,7 @@
       </c>
       <c r="Q35" s="27"/>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A36" s="100"/>
       <c r="B36">
         <v>1</v>
@@ -7923,7 +7968,7 @@
       <c r="P36" s="33"/>
       <c r="Q36" s="1"/>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="O37" s="30" t="s">
         <v>132</v>
       </c>
@@ -7932,7 +7977,7 @@
         <v>0.36551047740241704</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="O38" s="30" t="s">
         <v>133</v>
       </c>
@@ -7941,7 +7986,7 @@
         <v>0.14493952061648685</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="O39" s="30" t="s">
         <v>110</v>
       </c>
@@ -7950,7 +7995,7 @@
         <v>0.36551047740241704</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="O40" s="30" t="s">
         <v>111</v>
       </c>
@@ -7959,7 +8004,7 @@
         <v>0.14493952061648685</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="O42" s="30" t="s">
         <v>128</v>
       </c>
@@ -7968,7 +8013,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="O43" s="30" t="s">
         <v>127</v>
       </c>
@@ -7977,7 +8022,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
       <c r="O44" s="30" t="s">
         <v>131</v>
       </c>
@@ -8011,16 +8056,16 @@
       <selection activeCell="AK15" sqref="AK15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="12" bestFit="1" customWidth="1"/>
     <col min="46" max="48" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A1" s="49" t="s">
         <v>112</v>
       </c>
@@ -8034,7 +8079,7 @@
       <c r="W1" s="92"/>
       <c r="X1" s="93"/>
     </row>
-    <row r="2" spans="1:56" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:56" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="52" t="s">
         <v>112</v>
       </c>
@@ -8049,7 +8094,7 @@
       <c r="W2" s="94"/>
       <c r="X2" s="94"/>
     </row>
-    <row r="4" spans="1:56" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:56" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="98" t="s">
         <v>70</v>
       </c>
@@ -8217,7 +8262,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A5" s="98"/>
       <c r="B5">
         <v>1</v>
@@ -8412,7 +8457,7 @@
         <v>1.3244862745926676E-6</v>
       </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A6" s="98"/>
       <c r="B6">
         <v>1</v>
@@ -8607,7 +8652,7 @@
         <v>1.6879744031468265E-7</v>
       </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A7" s="98"/>
       <c r="B7">
         <v>1</v>
@@ -8799,7 +8844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A8" s="98"/>
       <c r="B8">
         <v>1</v>
@@ -8991,7 +9036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A9" s="98"/>
       <c r="B9">
         <v>1</v>
@@ -9183,7 +9228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A10" s="98"/>
       <c r="B10">
         <v>1</v>
@@ -9375,7 +9420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A11" s="98"/>
       <c r="B11">
         <v>1</v>
@@ -9567,7 +9612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A12" s="98"/>
       <c r="B12">
         <v>1</v>
@@ -9759,7 +9804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A13" s="98"/>
       <c r="B13">
         <f>B6</f>
@@ -9959,7 +10004,7 @@
       <c r="BC13" s="7"/>
       <c r="BD13" s="7"/>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A14" s="98"/>
       <c r="B14">
         <f t="shared" ref="B14:B19" si="27">B7</f>
@@ -10160,7 +10205,7 @@
       <c r="BC14" s="7"/>
       <c r="BD14" s="7"/>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A15" s="98"/>
       <c r="B15">
         <f t="shared" si="27"/>
@@ -10361,7 +10406,7 @@
       <c r="BC15" s="7"/>
       <c r="BD15" s="7"/>
     </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A16" s="98"/>
       <c r="B16">
         <f t="shared" si="27"/>
@@ -10562,7 +10607,7 @@
       <c r="BC16" s="7"/>
       <c r="BD16" s="7"/>
     </row>
-    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A17" s="98"/>
       <c r="B17">
         <f t="shared" si="27"/>
@@ -10763,7 +10808,7 @@
       <c r="BC17" s="7"/>
       <c r="BD17" s="7"/>
     </row>
-    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A18" s="98"/>
       <c r="B18">
         <f t="shared" si="27"/>
@@ -10964,7 +11009,7 @@
       <c r="BC18" s="7"/>
       <c r="BD18" s="7"/>
     </row>
-    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A19" s="98"/>
       <c r="B19">
         <f t="shared" si="27"/>
@@ -11165,7 +11210,7 @@
       <c r="BC19" s="7"/>
       <c r="BD19" s="7"/>
     </row>
-    <row r="20" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A20" s="98"/>
       <c r="B20">
         <f>B7</f>
@@ -11366,7 +11411,7 @@
       <c r="BC20" s="7"/>
       <c r="BD20" s="7"/>
     </row>
-    <row r="21" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A21" s="98"/>
       <c r="B21">
         <f t="shared" ref="B21:B34" si="67">B8</f>
@@ -11567,7 +11612,7 @@
       <c r="BC21" s="7"/>
       <c r="BD21" s="7"/>
     </row>
-    <row r="22" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A22" s="98"/>
       <c r="B22">
         <f t="shared" si="67"/>
@@ -11768,7 +11813,7 @@
       <c r="BC22" s="7"/>
       <c r="BD22" s="7"/>
     </row>
-    <row r="23" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A23" s="98"/>
       <c r="B23">
         <f t="shared" si="67"/>
@@ -11969,7 +12014,7 @@
       <c r="BC23" s="7"/>
       <c r="BD23" s="7"/>
     </row>
-    <row r="24" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A24" s="98"/>
       <c r="B24">
         <f t="shared" si="67"/>
@@ -12170,7 +12215,7 @@
       <c r="BC24" s="7"/>
       <c r="BD24" s="7"/>
     </row>
-    <row r="25" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A25" s="98"/>
       <c r="B25">
         <f t="shared" si="67"/>
@@ -12371,7 +12416,7 @@
       <c r="BC25" s="7"/>
       <c r="BD25" s="7"/>
     </row>
-    <row r="26" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A26" s="98"/>
       <c r="B26">
         <f t="shared" si="67"/>
@@ -12572,7 +12617,7 @@
       <c r="BC26" s="7"/>
       <c r="BD26" s="7"/>
     </row>
-    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A27" s="98"/>
       <c r="B27">
         <f t="shared" si="67"/>
@@ -12773,7 +12818,7 @@
       <c r="BC27" s="7"/>
       <c r="BD27" s="7"/>
     </row>
-    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A28" s="98"/>
       <c r="B28">
         <f t="shared" si="67"/>
@@ -12974,7 +13019,7 @@
       <c r="BC28" s="7"/>
       <c r="BD28" s="7"/>
     </row>
-    <row r="29" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A29" s="98"/>
       <c r="B29">
         <f t="shared" si="67"/>
@@ -13175,7 +13220,7 @@
       <c r="BC29" s="7"/>
       <c r="BD29" s="7"/>
     </row>
-    <row r="30" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A30" s="98"/>
       <c r="B30">
         <f t="shared" si="67"/>
@@ -13376,7 +13421,7 @@
       <c r="BC30" s="7"/>
       <c r="BD30" s="7"/>
     </row>
-    <row r="31" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A31" s="98"/>
       <c r="B31">
         <f t="shared" si="67"/>
@@ -13577,7 +13622,7 @@
       <c r="BC31" s="7"/>
       <c r="BD31" s="7"/>
     </row>
-    <row r="32" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A32" s="98"/>
       <c r="B32">
         <f t="shared" si="67"/>
@@ -13778,7 +13823,7 @@
       <c r="BC32" s="7"/>
       <c r="BD32" s="7"/>
     </row>
-    <row r="33" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A33" s="98"/>
       <c r="B33">
         <f t="shared" si="67"/>
@@ -13979,7 +14024,7 @@
       <c r="BC33" s="7"/>
       <c r="BD33" s="7"/>
     </row>
-    <row r="34" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A34" s="98"/>
       <c r="B34">
         <f t="shared" si="67"/>
@@ -14180,7 +14225,7 @@
       <c r="BC34" s="7"/>
       <c r="BD34" s="7"/>
     </row>
-    <row r="35" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="X35" s="1"/>
       <c r="Y35" s="1"/>
@@ -14192,7 +14237,7 @@
       <c r="AE35" s="1"/>
       <c r="AF35" s="1"/>
     </row>
-    <row r="36" spans="1:56" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:56" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="98" t="s">
         <v>71</v>
       </c>
@@ -14294,7 +14339,7 @@
       <c r="AU36" s="40"/>
       <c r="AV36" s="40"/>
     </row>
-    <row r="37" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A37" s="98"/>
       <c r="B37">
         <v>1</v>
@@ -14420,7 +14465,7 @@
       <c r="AU37" s="83"/>
       <c r="AV37" s="83"/>
     </row>
-    <row r="38" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A38" s="98"/>
       <c r="B38">
         <v>1</v>
@@ -14548,7 +14593,7 @@
       <c r="AU38" s="84"/>
       <c r="AV38" s="84"/>
     </row>
-    <row r="39" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A39" s="98"/>
       <c r="B39">
         <v>1</v>
@@ -14654,7 +14699,7 @@
       <c r="AF39" s="1"/>
       <c r="AG39" s="1"/>
     </row>
-    <row r="40" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A40" s="98"/>
       <c r="B40">
         <v>1</v>
@@ -14760,7 +14805,7 @@
       <c r="AF40" s="1"/>
       <c r="AG40" s="1"/>
     </row>
-    <row r="41" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A41" s="98"/>
       <c r="B41">
         <v>1</v>
@@ -14871,7 +14916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A42" s="98"/>
       <c r="B42">
         <v>1</v>
@@ -14979,7 +15024,7 @@
         <v>0.106</v>
       </c>
     </row>
-    <row r="43" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="W43" s="15"/>
       <c r="X43" s="15"/>
@@ -15000,7 +15045,7 @@
         <v>1.28</v>
       </c>
     </row>
-    <row r="44" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="V44" s="29"/>
       <c r="W44" s="80"/>
@@ -15032,7 +15077,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="45" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="X45" s="14">
         <f>INPUTS!X23</f>
@@ -15065,7 +15110,7 @@
         <v>1512000</v>
       </c>
     </row>
-    <row r="46" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -15085,7 +15130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A47" s="98" t="s">
         <v>72</v>
       </c>
@@ -15142,7 +15187,7 @@
         <v>1.6949152542372881E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A48" s="98"/>
       <c r="B48">
         <v>1</v>
@@ -15192,7 +15237,7 @@
       <c r="AV48" s="7"/>
       <c r="AW48" s="7"/>
     </row>
-    <row r="49" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A49" s="98"/>
       <c r="B49">
         <v>1</v>
@@ -15269,7 +15314,7 @@
       <c r="AV49" s="7"/>
       <c r="AW49" s="7"/>
     </row>
-    <row r="50" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:49" x14ac:dyDescent="0.3">
       <c r="E50" s="46">
         <f>AB38</f>
         <v>5882.3529411764703</v>
@@ -15328,7 +15373,7 @@
       <c r="AV50" s="7"/>
       <c r="AW50" s="7"/>
     </row>
-    <row r="51" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:49" x14ac:dyDescent="0.3">
       <c r="F51" s="1"/>
       <c r="R51" s="99"/>
       <c r="S51" s="7" t="s">
@@ -15357,7 +15402,7 @@
       <c r="AV51" s="7"/>
       <c r="AW51" s="7"/>
     </row>
-    <row r="52" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:49" x14ac:dyDescent="0.3">
       <c r="D52" s="23" t="s">
         <v>78</v>
       </c>
@@ -15394,7 +15439,7 @@
       <c r="AV52" s="7"/>
       <c r="AW52" s="7"/>
     </row>
-    <row r="53" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:49" x14ac:dyDescent="0.3">
       <c r="D53" s="20" t="s">
         <v>79</v>
       </c>
@@ -15442,7 +15487,7 @@
       <c r="AV53" s="7"/>
       <c r="AW53" s="7"/>
     </row>
-    <row r="54" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:49" x14ac:dyDescent="0.3">
       <c r="D54" s="20" t="s">
         <v>76</v>
       </c>
@@ -15476,7 +15521,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:49" x14ac:dyDescent="0.3">
       <c r="O55" s="30" t="s">
         <v>108</v>
       </c>
@@ -15491,7 +15536,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="56" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:49" x14ac:dyDescent="0.3">
       <c r="O56" s="30" t="s">
         <v>109</v>
       </c>
@@ -15500,7 +15545,7 @@
         <v>4.1819835162284831E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="101" t="s">
         <v>152</v>
       </c>
@@ -15549,7 +15594,7 @@
       </c>
       <c r="Q57" s="27"/>
     </row>
-    <row r="58" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A58" s="101"/>
       <c r="B58">
         <v>1</v>
@@ -15591,7 +15636,7 @@
       <c r="P58" s="33"/>
       <c r="Q58" s="1"/>
     </row>
-    <row r="59" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A59" s="101"/>
       <c r="B59">
         <f>B58</f>
@@ -15647,7 +15692,7 @@
         <v>0.41149313987517477</v>
       </c>
     </row>
-    <row r="60" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A60" s="101"/>
       <c r="B60">
         <f>B59</f>
@@ -15703,7 +15748,7 @@
         <v>0.17634374328200197</v>
       </c>
     </row>
-    <row r="61" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A61" s="101"/>
       <c r="B61">
         <f>B60</f>
@@ -15759,7 +15804,7 @@
         <v>0.41149313987517477</v>
       </c>
     </row>
-    <row r="62" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A62" s="101"/>
       <c r="B62">
         <f>B61</f>
@@ -15815,7 +15860,7 @@
         <v>0.17634374328200197</v>
       </c>
     </row>
-    <row r="64" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:49" x14ac:dyDescent="0.3">
       <c r="O64" s="30" t="s">
         <v>128</v>
       </c>
@@ -15824,7 +15869,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="65" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O65" s="30" t="s">
         <v>127</v>
       </c>
@@ -15833,7 +15878,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="66" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O66" s="30" t="s">
         <v>131</v>
       </c>
@@ -15863,17 +15908,17 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B1" s="90" t="s">
         <v>155</v>
       </c>
@@ -15893,7 +15938,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>154</v>
       </c>
@@ -15918,7 +15963,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>165</v>
       </c>
@@ -15944,7 +15989,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>156</v>
       </c>
@@ -15970,7 +16015,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E5" s="81"/>
     </row>
   </sheetData>
@@ -15987,14 +16032,14 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C3" s="26" t="s">
         <v>93</v>
       </c>
@@ -16014,7 +16059,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>97</v>
       </c>
@@ -16040,7 +16085,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>11</v>
       </c>
@@ -16068,7 +16113,7 @@
         <v>107.14285714285714</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10</v>
       </c>
@@ -16096,7 +16141,7 @@
         <v>88.888888888888886</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>9</v>
       </c>
@@ -16124,7 +16169,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -16152,7 +16197,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>11</v>
       </c>
@@ -16180,7 +16225,7 @@
         <v>4.0650406504065044</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10</v>
       </c>
@@ -16208,7 +16253,7 @@
         <v>2.1052631578947367</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -16236,7 +16281,7 @@
         <v>2.054794520547945</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>8</v>
       </c>
@@ -16264,7 +16309,7 @@
         <v>25.862068965517242</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -16292,7 +16337,7 @@
         <v>15.625</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>11</v>
       </c>
@@ -16320,7 +16365,7 @@
         <v>3.125</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10</v>
       </c>
@@ -16348,7 +16393,7 @@
         <v>0.98684210526315796</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>9</v>
       </c>
@@ -16376,7 +16421,7 @@
         <v>0.91743119266055051</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>8</v>
       </c>
@@ -16404,7 +16449,7 @@
         <v>1.3513513513513513</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>173</v>
       </c>
@@ -16414,7 +16459,7 @@
       <c r="F18" s="24"/>
       <c r="I18" s="24"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>174</v>
       </c>
@@ -16422,7 +16467,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>153</v>
       </c>
@@ -16443,7 +16488,7 @@
         <v>71.428571428571431</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>172</v>
       </c>
@@ -16452,7 +16497,7 @@
       </c>
       <c r="I21" s="24"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>106</v>
       </c>
@@ -16472,7 +16517,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>130</v>
       </c>
@@ -16495,9 +16540,9 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>175</v>
       </c>
@@ -16509,7 +16554,7 @@
         <v>6.666666666666667</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>176</v>
       </c>

</xml_diff>